<commit_message>
update NASDAQ ESG + returns
using iShares NASDAQ100 Index ETF, Lyxor Nasdaq 100, iShares NASDAQ 100 ETF (ETF) as filter
</commit_message>
<xml_diff>
--- a/raw_data/Returns_NASDAQ100_20Y.xlsx
+++ b/raw_data/Returns_NASDAQ100_20Y.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adby364\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F100D2D-A2A4-47A6-B98D-2045B3058259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5265D6B-C76B-4A66-B8EF-162C628FABA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unsaved Template" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029" forceFullCalc="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="232">
   <si>
     <t>Identifier</t>
   </si>
@@ -735,114 +738,6 @@
     <t>Exchange Name</t>
   </si>
   <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>NASDAQ/NGS (GLOBAL SELECT MARKET)</t>
-  </si>
-  <si>
-    <t>Semiconductors &amp; Semiconductor Equipment</t>
-  </si>
-  <si>
-    <t>Hotels, Restaurants &amp; Leisure</t>
-  </si>
-  <si>
-    <t>Interactive Media &amp; Services</t>
-  </si>
-  <si>
-    <t>Broadline Retail</t>
-  </si>
-  <si>
-    <t>Electric Utilities</t>
-  </si>
-  <si>
-    <t>Biotechnology</t>
-  </si>
-  <si>
-    <t>Technology Hardware, Storage &amp; Peripherals</t>
-  </si>
-  <si>
-    <t>Pharmaceuticals</t>
-  </si>
-  <si>
-    <t>Professional Services</t>
-  </si>
-  <si>
-    <t>Energy Equipment &amp; Services</t>
-  </si>
-  <si>
-    <t>Electronic Equipment, Instruments &amp; Components</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>Commercial Services &amp; Supplies</t>
-  </si>
-  <si>
-    <t>Communications Equipment</t>
-  </si>
-  <si>
-    <t>Beverages</t>
-  </si>
-  <si>
-    <t>IT Services</t>
-  </si>
-  <si>
-    <t>Real Estate Management &amp; Development</t>
-  </si>
-  <si>
-    <t>Consumer Staples Distribution &amp; Retail</t>
-  </si>
-  <si>
-    <t>Ground Transportation</t>
-  </si>
-  <si>
-    <t>Health Care Equipment &amp; Supplies</t>
-  </si>
-  <si>
-    <t>Oil, Gas &amp; Consumable Fuels</t>
-  </si>
-  <si>
-    <t>Entertainment</t>
-  </si>
-  <si>
-    <t>Trading Companies &amp; Distributors</t>
-  </si>
-  <si>
-    <t>Industrial Conglomerates</t>
-  </si>
-  <si>
-    <t>Life Sciences Tools &amp; Services</t>
-  </si>
-  <si>
-    <t>Food Products</t>
-  </si>
-  <si>
-    <t>Chemicals</t>
-  </si>
-  <si>
-    <t>Textiles, Apparel &amp; Luxury Goods</t>
-  </si>
-  <si>
-    <t>NASDAQ/NMS (GLOBAL MARKET)</t>
-  </si>
-  <si>
-    <t>Specialty Retail</t>
-  </si>
-  <si>
-    <t>Machinery</t>
-  </si>
-  <si>
-    <t>Financial Services</t>
-  </si>
-  <si>
-    <t>Wireless Telecommunication Services</t>
-  </si>
-  <si>
-    <t>Automobiles</t>
-  </si>
-  <si>
     <t>Total Liabilities
 (USD)
 In the last 20 FY</t>
@@ -933,6 +828,1485 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Current Screen Template"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Identifier</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>Company Name</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Exchange Name</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>GICS Industry Name</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>ADBE.OQ</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>Adobe Inc</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>AMD.OQ</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Advanced Micro Devices Inc</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>HON.OQ</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Honeywell International Inc</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>Industrial Conglomerates</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>AEP.OQ</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>American Electric Power Company Inc</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>Electric Utilities</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>AMGN.OQ</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>Amgen Inc</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>Biotechnology</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>ADI.OQ</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>Analog Devices Inc</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>AAPL.OQ</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>Apple Inc</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>Technology Hardware, Storage &amp; Peripherals</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>AMAT.OQ</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>Applied Materials Inc</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>ADSK.OQ</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>Autodesk Inc</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>ADP.OQ</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>Automatic Data Processing Inc</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>Professional Services</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>BKR.OQ</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>Baker Hughes Co</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>Energy Equipment &amp; Services</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>CSX.OQ</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>CSX Corp</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D13" t="str">
+            <v>Ground Transportation</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>CDNS.OQ</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>Cadence Design Systems Inc</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>CSCO.OQ</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>Cisco Systems Inc</v>
+          </cell>
+          <cell r="C15" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v>Communications Equipment</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>CTAS.OQ</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>Cintas Corp</v>
+          </cell>
+          <cell r="C16" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D16" t="str">
+            <v>Commercial Services &amp; Supplies</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>CCEP.OQ</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>Coca-Cola Europacific Partners PLC</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>Beverages</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>CPRT.OQ</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>Copart Inc</v>
+          </cell>
+          <cell r="C18" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D18" t="str">
+            <v>Commercial Services &amp; Supplies</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>EA.OQ</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>Electronic Arts Inc</v>
+          </cell>
+          <cell r="C19" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D19" t="str">
+            <v>Entertainment</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>FAST.OQ</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>Fastenal Co</v>
+          </cell>
+          <cell r="C20" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D20" t="str">
+            <v>Trading Companies &amp; Distributors</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>GILD.OQ</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>Gilead Sciences Inc</v>
+          </cell>
+          <cell r="C21" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D21" t="str">
+            <v>Biotechnology</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>BIIB.OQ</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>Biogen Inc</v>
+          </cell>
+          <cell r="C22" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D22" t="str">
+            <v>Biotechnology</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>IDXX.OQ</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>IDEXX Laboratories Inc</v>
+          </cell>
+          <cell r="C23" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D23" t="str">
+            <v>Health Care Equipment &amp; Supplies</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>INTC.OQ</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>Intel Corp</v>
+          </cell>
+          <cell r="C24" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D24" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>INTU.OQ</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>Intuit Inc</v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D25" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>KLAC.OQ</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>KLA Corp</v>
+          </cell>
+          <cell r="C26" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>LRCX.OQ</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>Lam Research Corp</v>
+          </cell>
+          <cell r="C27" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>MAR.OQ</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>Marriott International Inc</v>
+          </cell>
+          <cell r="C28" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v>Hotels, Restaurants &amp; Leisure</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>MSFT.OQ</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>Microsoft Corp</v>
+          </cell>
+          <cell r="C29" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D29" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>MCHP.OQ</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>Microchip Technology Inc</v>
+          </cell>
+          <cell r="C30" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D30" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>MU.OQ</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>Micron Technology Inc</v>
+          </cell>
+          <cell r="C31" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D31" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>XEL.OQ</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>Xcel Energy Inc</v>
+          </cell>
+          <cell r="C32" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D32" t="str">
+            <v>Electric Utilities</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>ODFL.OQ</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>Old Dominion Freight Line Inc</v>
+          </cell>
+          <cell r="C33" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D33" t="str">
+            <v>Ground Transportation</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>ORLY.OQ</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>O'Reilly Automotive Inc</v>
+          </cell>
+          <cell r="C34" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D34" t="str">
+            <v>Specialty Retail</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>EXC.OQ</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>Exelon Corp</v>
+          </cell>
+          <cell r="C35" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D35" t="str">
+            <v>Electric Utilities</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>PCAR.OQ</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>Paccar Inc</v>
+          </cell>
+          <cell r="C36" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v>Machinery</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>PAYX.OQ</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>Paychex Inc</v>
+          </cell>
+          <cell r="C37" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D37" t="str">
+            <v>Professional Services</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>PEP.OQ</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>PepsiCo Inc</v>
+          </cell>
+          <cell r="C38" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D38" t="str">
+            <v>Beverages</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>QCOM.OQ</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>Qualcomm Inc</v>
+          </cell>
+          <cell r="C39" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>REGN.OQ</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>Regeneron Pharmaceuticals Inc</v>
+          </cell>
+          <cell r="C40" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D40" t="str">
+            <v>Biotechnology</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>ROP.OQ</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>Roper Technologies Inc</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>ROST.OQ</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>Ross Stores Inc</v>
+          </cell>
+          <cell r="C42" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D42" t="str">
+            <v>Specialty Retail</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>SBUX.OQ</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>Starbucks Corp</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D43" t="str">
+            <v>Hotels, Restaurants &amp; Leisure</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>SNPS.OQ</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>Synopsys Inc</v>
+          </cell>
+          <cell r="C44" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D44" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>TXN.OQ</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>Texas Instruments Inc</v>
+          </cell>
+          <cell r="C45" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D45" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>VRTX.OQ</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>Vertex Pharmaceuticals Inc</v>
+          </cell>
+          <cell r="C46" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D46" t="str">
+            <v>Biotechnology</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>AZN.OQ</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>AstraZeneca PLC</v>
+          </cell>
+          <cell r="C47" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D47" t="str">
+            <v>Pharmaceuticals</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>ASML.OQ</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>ASML Holding NV</v>
+          </cell>
+          <cell r="C48" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D48" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>AMZN.OQ</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>Amazon.com Inc</v>
+          </cell>
+          <cell r="C49" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D49" t="str">
+            <v>Broadline Retail</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>CTSH.OQ</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>Cognizant Technology Solutions Corp</v>
+          </cell>
+          <cell r="C50" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D50" t="str">
+            <v>IT Services</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>NVDA.OQ</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>NVIDIA Corp</v>
+          </cell>
+          <cell r="C51" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D51" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>BKNG.OQ</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>Booking Holdings Inc</v>
+          </cell>
+          <cell r="C52" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D52" t="str">
+            <v>Hotels, Restaurants &amp; Leisure</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>CSGP.OQ</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>CoStar Group Inc</v>
+          </cell>
+          <cell r="C53" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D53" t="str">
+            <v>Real Estate Management &amp; Development</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>COST.OQ</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>Costco Wholesale Corp</v>
+          </cell>
+          <cell r="C54" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D54" t="str">
+            <v>Consumer Staples Distribution &amp; Retail</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>TTWO.OQ</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>Take-Two Interactive Software Inc</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D55" t="str">
+            <v>Entertainment</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>ON.OQ</v>
+          </cell>
+          <cell r="B56" t="str">
+            <v>ON Semiconductor Corp</v>
+          </cell>
+          <cell r="C56" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D56" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57" t="str">
+            <v>ANSS.OQ</v>
+          </cell>
+          <cell r="B57" t="str">
+            <v>ANSYS Inc</v>
+          </cell>
+          <cell r="C57" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D57" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58" t="str">
+            <v>ILMN.OQ</v>
+          </cell>
+          <cell r="B58" t="str">
+            <v>Illumina Inc</v>
+          </cell>
+          <cell r="C58" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D58" t="str">
+            <v>Life Sciences Tools &amp; Services</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>ISRG.OQ</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v>Intuitive Surgical Inc</v>
+          </cell>
+          <cell r="C59" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D59" t="str">
+            <v>Health Care Equipment &amp; Supplies</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>MNST.OQ</v>
+          </cell>
+          <cell r="B60" t="str">
+            <v>Monster Beverage Corp</v>
+          </cell>
+          <cell r="C60" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D60" t="str">
+            <v>Beverages</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>MDLZ.OQ</v>
+          </cell>
+          <cell r="B61" t="str">
+            <v>Mondelez International Inc</v>
+          </cell>
+          <cell r="C61" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D61" t="str">
+            <v>Food Products</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>MRVL.OQ</v>
+          </cell>
+          <cell r="B62" t="str">
+            <v>Marvell Technology Inc</v>
+          </cell>
+          <cell r="C62" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D62" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>NFLX.OQ</v>
+          </cell>
+          <cell r="B63" t="str">
+            <v>Netflix Inc</v>
+          </cell>
+          <cell r="C63" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D63" t="str">
+            <v>Entertainment</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>CMCSA.OQ</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v>Comcast Corp</v>
+          </cell>
+          <cell r="C64" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D64" t="str">
+            <v>Media</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>TMUS.OQ</v>
+          </cell>
+          <cell r="B65" t="str">
+            <v>T-Mobile US Inc</v>
+          </cell>
+          <cell r="C65" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D65" t="str">
+            <v>Wireless Telecommunication Services</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>GOOGL.OQ</v>
+          </cell>
+          <cell r="B66" t="str">
+            <v>Alphabet Inc</v>
+          </cell>
+          <cell r="C66" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D66" t="str">
+            <v>Interactive Media &amp; Services</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>DXCM.OQ</v>
+          </cell>
+          <cell r="B67" t="str">
+            <v>Dexcom Inc</v>
+          </cell>
+          <cell r="C67" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D67" t="str">
+            <v>Health Care Equipment &amp; Supplies</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>LULU.OQ</v>
+          </cell>
+          <cell r="B68" t="str">
+            <v>Lululemon Athletica Inc</v>
+          </cell>
+          <cell r="C68" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D68" t="str">
+            <v>Textiles, Apparel &amp; Luxury Goods</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>MELI.OQ</v>
+          </cell>
+          <cell r="B69" t="str">
+            <v>MercadoLibre Inc</v>
+          </cell>
+          <cell r="C69" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D69" t="str">
+            <v>Broadline Retail</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>KDP.OQ</v>
+          </cell>
+          <cell r="B70" t="str">
+            <v>Keurig Dr Pepper Inc</v>
+          </cell>
+          <cell r="C70" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D70" t="str">
+            <v>Beverages</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71" t="str">
+            <v>WBD.OQ</v>
+          </cell>
+          <cell r="B71" t="str">
+            <v>Warner Bros Discovery Inc</v>
+          </cell>
+          <cell r="C71" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D71" t="str">
+            <v>Entertainment</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72" t="str">
+            <v>AVGO.OQ</v>
+          </cell>
+          <cell r="B72" t="str">
+            <v>Broadcom Inc</v>
+          </cell>
+          <cell r="C72" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D72" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>VRSK.OQ</v>
+          </cell>
+          <cell r="B73" t="str">
+            <v>Verisk Analytics Inc</v>
+          </cell>
+          <cell r="C73" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D73" t="str">
+            <v>Professional Services</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>FTNT.OQ</v>
+          </cell>
+          <cell r="B74" t="str">
+            <v>Fortinet Inc</v>
+          </cell>
+          <cell r="C74" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D74" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>CHTR.OQ</v>
+          </cell>
+          <cell r="B75" t="str">
+            <v>Charter Communications Inc</v>
+          </cell>
+          <cell r="C75" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D75" t="str">
+            <v>Media</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>TSLA.OQ</v>
+          </cell>
+          <cell r="B76" t="str">
+            <v>Tesla Inc</v>
+          </cell>
+          <cell r="C76" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D76" t="str">
+            <v>Automobiles</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>NXPI.OQ</v>
+          </cell>
+          <cell r="B77" t="str">
+            <v>NXP Semiconductors NV</v>
+          </cell>
+          <cell r="C77" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D77" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>META.OQ</v>
+          </cell>
+          <cell r="B78" t="str">
+            <v>Meta Platforms Inc</v>
+          </cell>
+          <cell r="C78" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D78" t="str">
+            <v>Interactive Media &amp; Services</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>FANG.OQ</v>
+          </cell>
+          <cell r="B79" t="str">
+            <v>Diamondback Energy Inc</v>
+          </cell>
+          <cell r="C79" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D79" t="str">
+            <v>Oil, Gas &amp; Consumable Fuels</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>PANW.OQ</v>
+          </cell>
+          <cell r="B80" t="str">
+            <v>Palo Alto Networks Inc</v>
+          </cell>
+          <cell r="C80" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D80" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>WDAY.OQ</v>
+          </cell>
+          <cell r="B81" t="str">
+            <v>Workday Inc</v>
+          </cell>
+          <cell r="C81" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D81" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>CDW.OQ</v>
+          </cell>
+          <cell r="B82" t="str">
+            <v>CDW Corp</v>
+          </cell>
+          <cell r="C82" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D82" t="str">
+            <v>Electronic Equipment, Instruments &amp; Components</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>GOOG.OQ</v>
+          </cell>
+          <cell r="B83" t="str">
+            <v>Alphabet Inc</v>
+          </cell>
+          <cell r="C83" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D83" t="str">
+            <v>Interactive Media &amp; Services</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>KHC.OQ</v>
+          </cell>
+          <cell r="B84" t="str">
+            <v>Kraft Heinz Co</v>
+          </cell>
+          <cell r="C84" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D84" t="str">
+            <v>Food Products</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>PYPL.OQ</v>
+          </cell>
+          <cell r="B85" t="str">
+            <v>PayPal Holdings Inc</v>
+          </cell>
+          <cell r="C85" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D85" t="str">
+            <v>Financial Services</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86" t="str">
+            <v>TEAM.OQ</v>
+          </cell>
+          <cell r="B86" t="str">
+            <v>Atlassian Corp</v>
+          </cell>
+          <cell r="C86" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D86" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87" t="str">
+            <v>TTD.OQ</v>
+          </cell>
+          <cell r="B87" t="str">
+            <v>Trade Desk Inc</v>
+          </cell>
+          <cell r="C87" t="str">
+            <v>NASDAQ/NMS (GLOBAL MARKET)</v>
+          </cell>
+          <cell r="D87" t="str">
+            <v>Media</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88" t="str">
+            <v>MDB.OQ</v>
+          </cell>
+          <cell r="B88" t="str">
+            <v>MongoDB Inc</v>
+          </cell>
+          <cell r="C88" t="str">
+            <v>NASDAQ/NMS (GLOBAL MARKET)</v>
+          </cell>
+          <cell r="D88" t="str">
+            <v>IT Services</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89" t="str">
+            <v>ZS.OQ</v>
+          </cell>
+          <cell r="B89" t="str">
+            <v>Zscaler Inc</v>
+          </cell>
+          <cell r="C89" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D89" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90" t="str">
+            <v>PDD.OQ</v>
+          </cell>
+          <cell r="B90" t="str">
+            <v>PDD Holdings Inc</v>
+          </cell>
+          <cell r="C90" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D90" t="str">
+            <v>Broadline Retail</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91" t="str">
+            <v>LIN.OQ</v>
+          </cell>
+          <cell r="B91" t="str">
+            <v>Linde PLC</v>
+          </cell>
+          <cell r="C91" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D91" t="str">
+            <v>Chemicals</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92" t="str">
+            <v>MRNA.OQ</v>
+          </cell>
+          <cell r="B92" t="str">
+            <v>Moderna Inc</v>
+          </cell>
+          <cell r="C92" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D92" t="str">
+            <v>Biotechnology</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93" t="str">
+            <v>CRWD.OQ</v>
+          </cell>
+          <cell r="B93" t="str">
+            <v>CrowdStrike Holdings Inc</v>
+          </cell>
+          <cell r="C93" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D93" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94" t="str">
+            <v>DDOG.OQ</v>
+          </cell>
+          <cell r="B94" t="str">
+            <v>Datadog Inc</v>
+          </cell>
+          <cell r="C94" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D94" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95" t="str">
+            <v>SMCI.OQ</v>
+          </cell>
+          <cell r="B95" t="str">
+            <v>Super Micro Computer Inc</v>
+          </cell>
+          <cell r="C95" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D95" t="str">
+            <v>Technology Hardware, Storage &amp; Peripherals</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96" t="str">
+            <v>ABNB.OQ</v>
+          </cell>
+          <cell r="B96" t="str">
+            <v>Airbnb Inc</v>
+          </cell>
+          <cell r="C96" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D96" t="str">
+            <v>Hotels, Restaurants &amp; Leisure</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97" t="str">
+            <v>DASH.OQ</v>
+          </cell>
+          <cell r="B97" t="str">
+            <v>DoorDash Inc</v>
+          </cell>
+          <cell r="C97" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D97" t="str">
+            <v>Hotels, Restaurants &amp; Leisure</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98" t="str">
+            <v>APP.OQ</v>
+          </cell>
+          <cell r="B98" t="str">
+            <v>Applovin Corp</v>
+          </cell>
+          <cell r="C98" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D98" t="str">
+            <v>Software</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99" t="str">
+            <v>GFS.OQ</v>
+          </cell>
+          <cell r="B99" t="str">
+            <v>GlobalFoundries Inc</v>
+          </cell>
+          <cell r="C99" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D99" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100" t="str">
+            <v>CEG.OQ</v>
+          </cell>
+          <cell r="B100" t="str">
+            <v>Constellation Energy Corp</v>
+          </cell>
+          <cell r="C100" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D100" t="str">
+            <v>Electric Utilities</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101" t="str">
+            <v>GEHC.OQ</v>
+          </cell>
+          <cell r="B101" t="str">
+            <v>GE Healthcare Technologies Inc</v>
+          </cell>
+          <cell r="C101" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D101" t="str">
+            <v>Health Care Equipment &amp; Supplies</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102" t="str">
+            <v>ARM.OQ</v>
+          </cell>
+          <cell r="B102" t="str">
+            <v>Arm Holdings PLC</v>
+          </cell>
+          <cell r="C102" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D102" t="str">
+            <v>Semiconductors &amp; Semiconductor Equipment</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103" t="str">
+            <v>.ONEHKD</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104" t="str">
+            <v>.ONEUSD</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105" t="str">
+            <v>DLTR.OQ</v>
+          </cell>
+          <cell r="B105" t="str">
+            <v>Dollar Tree Inc</v>
+          </cell>
+          <cell r="C105" t="str">
+            <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
+          </cell>
+          <cell r="D105" t="str">
+            <v>Consumer Staples Distribution &amp; Retail</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106" t="str">
+            <v>MQNZ24</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107" t="str">
+            <v>.ONECAD</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1227,8 +2601,8 @@
   </sheetPr>
   <dimension ref="A1:GV106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EH1" workbookViewId="0">
-      <selection activeCell="ES12" sqref="ES12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,7 +3048,7 @@
         <v>3</v>
       </c>
       <c r="EO1" s="5" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="EP1" s="5" t="s">
         <v>3</v>
@@ -1734,7 +3108,7 @@
         <v>3</v>
       </c>
       <c r="FI1" s="5" t="s">
-        <v>267</v>
+        <v>231</v>
       </c>
       <c r="FJ1" s="5" t="s">
         <v>3</v>
@@ -2468,11 +3842,13 @@
       <c r="B4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>231</v>
+      <c r="C4" s="2" t="str">
+        <f>VLOOKUP(A4,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>VLOOKUP(A4,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E4" s="3">
         <v>0.48259000000000002</v>
@@ -2996,11 +4372,13 @@
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>231</v>
+      <c r="C5" s="2" t="str">
+        <f>VLOOKUP(A5,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>VLOOKUP(A5,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E5" s="3">
         <v>7.7800000000000008E-2</v>
@@ -3522,11 +4900,13 @@
       <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>231</v>
+      <c r="C6" s="2" t="str">
+        <f>VLOOKUP(A6,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Hotels, Restaurants &amp; Leisure</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>VLOOKUP(A6,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E6" s="3">
         <v>0.82040000000000002</v>
@@ -3814,11 +5194,13 @@
       <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>231</v>
+      <c r="C7" s="2" t="str">
+        <f>VLOOKUP(A7,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Interactive Media &amp; Services</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>VLOOKUP(A7,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E7" s="3">
         <v>0.27359</v>
@@ -4282,11 +5664,13 @@
       <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>231</v>
+      <c r="C8" s="2" t="str">
+        <f>VLOOKUP(A8,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Interactive Media &amp; Services</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>VLOOKUP(A8,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E8" s="3">
         <v>0.27359</v>
@@ -4812,11 +6196,13 @@
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>231</v>
+      <c r="C9" s="2" t="str">
+        <f>VLOOKUP(A9,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Broadline Retail</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>VLOOKUP(A9,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E9" s="3">
         <v>0.17489000000000002</v>
@@ -5342,11 +6728,13 @@
       <c r="B10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>231</v>
+      <c r="C10" s="2" t="str">
+        <f>VLOOKUP(A10,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Electric Utilities</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>VLOOKUP(A10,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E10" s="3">
         <v>0.1108</v>
@@ -5906,11 +7294,13 @@
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>231</v>
+      <c r="C11" s="2" t="str">
+        <f>VLOOKUP(A11,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Biotechnology</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>VLOOKUP(A11,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E11" s="3">
         <v>2.0284899999999997</v>
@@ -6440,11 +7830,13 @@
       <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>231</v>
+      <c r="C12" s="2" t="str">
+        <f>VLOOKUP(A12,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>VLOOKUP(A12,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E12" s="3">
         <v>0.14169000000000001</v>
@@ -6976,11 +8368,13 @@
       <c r="B13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>231</v>
+      <c r="C13" s="2" t="str">
+        <f>VLOOKUP(A13,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>VLOOKUP(A13,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E13" s="3">
         <v>0.15</v>
@@ -7506,11 +8900,13 @@
       <c r="B14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>231</v>
+      <c r="C14" s="2" t="str">
+        <f>VLOOKUP(A14,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Technology Hardware, Storage &amp; Peripherals</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>VLOOKUP(A14,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E14" s="3">
         <v>1.7462</v>
@@ -8038,11 +9434,13 @@
       <c r="B15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>231</v>
+      <c r="C15" s="2" t="str">
+        <f>VLOOKUP(A15,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f>VLOOKUP(A15,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E15" s="3">
         <v>0.47659000000000001</v>
@@ -8568,11 +9966,13 @@
       <c r="B16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>231</v>
+      <c r="C16" s="2" t="str">
+        <f>VLOOKUP(A16,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>VLOOKUP(A16,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E16" s="3">
         <v>0.2833</v>
@@ -8806,11 +10206,13 @@
       <c r="B17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>231</v>
+      <c r="C17" s="2" t="str">
+        <f>VLOOKUP(A17,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>VLOOKUP(A17,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E17" s="3">
         <v>0.70421000000000011</v>
@@ -9322,11 +10724,13 @@
       <c r="B18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>231</v>
+      <c r="C18" s="2" t="str">
+        <f>VLOOKUP(A18,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Pharmaceuticals</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f>VLOOKUP(A18,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E18" s="3">
         <v>0.38159999999999994</v>
@@ -9886,11 +11290,13 @@
       <c r="B19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>231</v>
+      <c r="C19" s="2" t="str">
+        <f>VLOOKUP(A19,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f>VLOOKUP(A19,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E19" s="3">
         <v>0.90358999999999989</v>
@@ -10214,11 +11620,13 @@
       <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>231</v>
+      <c r="C20" s="2" t="str">
+        <f>VLOOKUP(A20,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f>VLOOKUP(A20,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E20" s="3">
         <v>1.09439</v>
@@ -10734,11 +12142,13 @@
       <c r="B21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>231</v>
+      <c r="C21" s="2" t="str">
+        <f>VLOOKUP(A21,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Professional Services</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f>VLOOKUP(A21,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E21" s="3">
         <v>0.9395</v>
@@ -11258,11 +12668,13 @@
       <c r="B22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>231</v>
+      <c r="C22" s="2" t="str">
+        <f>VLOOKUP(A22,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Energy Equipment &amp; Services</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f>VLOOKUP(A22,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E22" s="3">
         <v>0.10839</v>
@@ -11802,11 +13214,13 @@
       <c r="B23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>231</v>
+      <c r="C23" s="2" t="str">
+        <f>VLOOKUP(A23,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Biotechnology</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f>VLOOKUP(A23,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E23" s="3">
         <v>0.15210000000000001</v>
@@ -12366,11 +13780,13 @@
       <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>231</v>
+      <c r="C24" s="2" t="str">
+        <f>VLOOKUP(A24,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Hotels, Restaurants &amp; Leisure</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f>VLOOKUP(A24,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3">
@@ -12912,11 +14328,13 @@
       <c r="B25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>231</v>
+      <c r="C25" s="2" t="str">
+        <f>VLOOKUP(A25,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f>VLOOKUP(A25,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E25" s="3">
         <v>0.78709000000000007</v>
@@ -13354,11 +14772,13 @@
       <c r="B26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>231</v>
+      <c r="C26" s="2" t="str">
+        <f>VLOOKUP(A26,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f>VLOOKUP(A26,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E26" s="3">
         <v>0.45679000000000003</v>
@@ -13870,11 +15290,13 @@
       <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>231</v>
+      <c r="C27" s="2" t="str">
+        <f>VLOOKUP(A27,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Electronic Equipment, Instruments &amp; Components</v>
+      </c>
+      <c r="D27" s="2" t="str">
+        <f>VLOOKUP(A27,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E27" s="3">
         <v>0.4733</v>
@@ -14306,11 +15728,13 @@
       <c r="B28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>231</v>
+      <c r="C28" s="2" t="str">
+        <f>VLOOKUP(A28,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Media</v>
+      </c>
+      <c r="D28" s="2" t="str">
+        <f>VLOOKUP(A28,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E28" s="3">
         <v>0.45108999999999999</v>
@@ -14758,11 +16182,13 @@
       <c r="B29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>231</v>
+      <c r="C29" s="2" t="str">
+        <f>VLOOKUP(A29,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Commercial Services &amp; Supplies</v>
+      </c>
+      <c r="D29" s="2" t="str">
+        <f>VLOOKUP(A29,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E29" s="3">
         <v>0.38420000000000004</v>
@@ -15290,11 +16716,13 @@
       <c r="B30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>231</v>
+      <c r="C30" s="2" t="str">
+        <f>VLOOKUP(A30,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Communications Equipment</v>
+      </c>
+      <c r="D30" s="2" t="str">
+        <f>VLOOKUP(A30,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E30" s="3">
         <v>0.33740000000000003</v>
@@ -15812,11 +17240,13 @@
       <c r="B31" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>231</v>
+      <c r="C31" s="2" t="str">
+        <f>VLOOKUP(A31,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Beverages</v>
+      </c>
+      <c r="D31" s="2" t="str">
+        <f>VLOOKUP(A31,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E31" s="3">
         <v>0.22059999999999999</v>
@@ -16342,11 +17772,13 @@
       <c r="B32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>231</v>
+      <c r="C32" s="2" t="str">
+        <f>VLOOKUP(A32,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>IT Services</v>
+      </c>
+      <c r="D32" s="2" t="str">
+        <f>VLOOKUP(A32,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E32" s="3">
         <v>0.18</v>
@@ -16876,11 +18308,13 @@
       <c r="B33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>231</v>
+      <c r="C33" s="2" t="str">
+        <f>VLOOKUP(A33,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Media</v>
+      </c>
+      <c r="D33" s="2" t="str">
+        <f>VLOOKUP(A33,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E33" s="3">
         <v>0.2016</v>
@@ -17448,11 +18882,13 @@
       <c r="B34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>231</v>
+      <c r="C34" s="2" t="str">
+        <f>VLOOKUP(A34,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Electric Utilities</v>
+      </c>
+      <c r="D34" s="2" t="str">
+        <f>VLOOKUP(A34,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E34" s="3">
         <v>8.7300000000000003E-2</v>
@@ -17710,11 +19146,13 @@
       <c r="B35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>231</v>
+      <c r="C35" s="2" t="str">
+        <f>VLOOKUP(A35,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Commercial Services &amp; Supplies</v>
+      </c>
+      <c r="D35" s="2" t="str">
+        <f>VLOOKUP(A35,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E35" s="3">
         <v>0.20180000000000001</v>
@@ -18234,11 +19672,13 @@
       <c r="B36" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>231</v>
+      <c r="C36" s="2" t="str">
+        <f>VLOOKUP(A36,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Real Estate Management &amp; Development</v>
+      </c>
+      <c r="D36" s="2" t="str">
+        <f>VLOOKUP(A36,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E36" s="3">
         <v>7.009E-2</v>
@@ -18756,11 +20196,13 @@
       <c r="B37" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>231</v>
+      <c r="C37" s="2" t="str">
+        <f>VLOOKUP(A37,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Consumer Staples Distribution &amp; Retail</v>
+      </c>
+      <c r="D37" s="2" t="str">
+        <f>VLOOKUP(A37,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E37" s="3">
         <v>0.30268999999999996</v>
@@ -19312,11 +20754,13 @@
       <c r="B38" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>231</v>
+      <c r="C38" s="2" t="str">
+        <f>VLOOKUP(A38,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D38" s="2" t="str">
+        <f>VLOOKUP(A38,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E38" s="3">
         <v>0.39909</v>
@@ -19614,11 +21058,13 @@
       <c r="B39" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>231</v>
+      <c r="C39" s="2" t="str">
+        <f>VLOOKUP(A39,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Ground Transportation</v>
+      </c>
+      <c r="D39" s="2" t="str">
+        <f>VLOOKUP(A39,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E39" s="3">
         <v>0.30010000000000003</v>
@@ -20146,11 +21592,13 @@
       <c r="B40" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>231</v>
+      <c r="C40" s="2" t="str">
+        <f>VLOOKUP(A40,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D40" s="2" t="str">
+        <f>VLOOKUP(A40,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E40" s="3">
         <v>0.33509</v>
@@ -20434,11 +21882,13 @@
       <c r="B41" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>231</v>
+      <c r="C41" s="2" t="str">
+        <f>VLOOKUP(A41,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Health Care Equipment &amp; Supplies</v>
+      </c>
+      <c r="D41" s="2" t="str">
+        <f>VLOOKUP(A41,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E41" s="3">
         <v>0.29210000000000003</v>
@@ -20868,11 +22318,13 @@
       <c r="B42" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>231</v>
+      <c r="C42" s="2" t="str">
+        <f>VLOOKUP(A42,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Oil, Gas &amp; Consumable Fuels</v>
+      </c>
+      <c r="D42" s="2" t="str">
+        <f>VLOOKUP(A42,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E42" s="3">
         <v>0.2064</v>
@@ -21282,11 +22734,13 @@
       <c r="B43" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>231</v>
+      <c r="C43" s="2" t="str">
+        <f>VLOOKUP(A43,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Consumer Staples Distribution &amp; Retail</v>
+      </c>
+      <c r="D43" s="2" t="str">
+        <f>VLOOKUP(A43,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E43" s="3">
         <v>0.16059000000000001</v>
@@ -21808,11 +23262,13 @@
       <c r="B44" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>231</v>
+      <c r="C44" s="2" t="str">
+        <f>VLOOKUP(A44,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Hotels, Restaurants &amp; Leisure</v>
+      </c>
+      <c r="D44" s="2" t="str">
+        <f>VLOOKUP(A44,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E44" s="3">
         <v>-0.32919999999999999</v>
@@ -22088,11 +23544,13 @@
       <c r="B45" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>231</v>
+      <c r="C45" s="2" t="str">
+        <f>VLOOKUP(A45,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Entertainment</v>
+      </c>
+      <c r="D45" s="2" t="str">
+        <f>VLOOKUP(A45,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E45" s="3">
         <v>0.25420000000000004</v>
@@ -22614,11 +24072,13 @@
       <c r="B46" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>231</v>
+      <c r="C46" s="2" t="str">
+        <f>VLOOKUP(A46,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Electric Utilities</v>
+      </c>
+      <c r="D46" s="2" t="str">
+        <f>VLOOKUP(A46,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E46" s="3">
         <v>9.4100000000000003E-2</v>
@@ -23172,11 +24632,13 @@
       <c r="B47" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>231</v>
+      <c r="C47" s="2" t="str">
+        <f>VLOOKUP(A47,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Trading Companies &amp; Distributors</v>
+      </c>
+      <c r="D47" s="2" t="str">
+        <f>VLOOKUP(A47,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E47" s="3">
         <v>0.35469000000000001</v>
@@ -23698,11 +25160,13 @@
       <c r="B48" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>231</v>
+      <c r="C48" s="2" t="str">
+        <f>VLOOKUP(A48,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D48" s="2" t="str">
+        <f>VLOOKUP(A48,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E48" s="3">
         <v>-3.4512900000000002</v>
@@ -24140,11 +25604,13 @@
       <c r="B49" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>231</v>
+      <c r="C49" s="2" t="str">
+        <f>VLOOKUP(A49,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Health Care Equipment &amp; Supplies</v>
+      </c>
+      <c r="D49" s="2" t="str">
+        <f>VLOOKUP(A49,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E49" s="3">
         <v>0.2177</v>
@@ -24394,11 +25860,13 @@
       <c r="B50" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>231</v>
+      <c r="C50" s="2" t="str">
+        <f>VLOOKUP(A50,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Biotechnology</v>
+      </c>
+      <c r="D50" s="2" t="str">
+        <f>VLOOKUP(A50,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E50" s="3">
         <v>0.3846</v>
@@ -24958,11 +26426,13 @@
       <c r="B51" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>231</v>
+      <c r="C51" s="2" t="str">
+        <f>VLOOKUP(A51,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D51" s="2" t="str">
+        <f>VLOOKUP(A51,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E51" s="3">
         <v>0.11900000000000001</v>
@@ -25236,11 +26706,13 @@
       <c r="B52" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>231</v>
+      <c r="C52" s="2" t="str">
+        <f>VLOOKUP(A52,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Industrial Conglomerates</v>
+      </c>
+      <c r="D52" s="2" t="str">
+        <f>VLOOKUP(A52,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E52" s="3">
         <v>0.36259000000000002</v>
@@ -25786,11 +27258,13 @@
       <c r="B53" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>231</v>
+      <c r="C53" s="2" t="str">
+        <f>VLOOKUP(A53,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Health Care Equipment &amp; Supplies</v>
+      </c>
+      <c r="D53" s="2" t="str">
+        <f>VLOOKUP(A53,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E53" s="3">
         <v>0.80739000000000005</v>
@@ -26346,11 +27820,13 @@
       <c r="B54" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>231</v>
+      <c r="C54" s="2" t="str">
+        <f>VLOOKUP(A54,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Life Sciences Tools &amp; Services</v>
+      </c>
+      <c r="D54" s="2" t="str">
+        <f>VLOOKUP(A54,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E54" s="3">
         <v>2.2200000000000001E-2</v>
@@ -26876,11 +28352,13 @@
       <c r="B55" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>231</v>
+      <c r="C55" s="2" t="str">
+        <f>VLOOKUP(A55,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D55" s="2" t="str">
+        <f>VLOOKUP(A55,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E55" s="3">
         <v>4.2689999999999999E-2</v>
@@ -27408,11 +28886,13 @@
       <c r="B56" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>231</v>
+      <c r="C56" s="2" t="str">
+        <f>VLOOKUP(A56,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D56" s="2" t="str">
+        <f>VLOOKUP(A56,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E56" s="3">
         <v>0.26949000000000001</v>
@@ -27948,11 +29428,13 @@
       <c r="B57" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>231</v>
+      <c r="C57" s="2" t="str">
+        <f>VLOOKUP(A57,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Health Care Equipment &amp; Supplies</v>
+      </c>
+      <c r="D57" s="2" t="str">
+        <f>VLOOKUP(A57,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E57" s="3">
         <v>0.1671</v>
@@ -28496,11 +29978,13 @@
       <c r="B58" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>231</v>
+      <c r="C58" s="2" t="str">
+        <f>VLOOKUP(A58,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Beverages</v>
+      </c>
+      <c r="D58" s="2" t="str">
+        <f>VLOOKUP(A58,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E58" s="3">
         <v>9.9100000000000008E-2</v>
@@ -28962,11 +30446,13 @@
       <c r="B59" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>231</v>
+      <c r="C59" s="2" t="str">
+        <f>VLOOKUP(A59,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D59" s="2" t="str">
+        <f>VLOOKUP(A59,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E59" s="3">
         <v>1.0284900000000001</v>
@@ -29516,11 +31002,13 @@
       <c r="B60" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>231</v>
+      <c r="C60" s="2" t="str">
+        <f>VLOOKUP(A60,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Food Products</v>
+      </c>
+      <c r="D60" s="2" t="str">
+        <f>VLOOKUP(A60,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E60" s="3">
         <v>7.4499999999999997E-2</v>
@@ -29898,11 +31386,13 @@
       <c r="B61" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>231</v>
+      <c r="C61" s="2" t="str">
+        <f>VLOOKUP(A61,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D61" s="2" t="str">
+        <f>VLOOKUP(A61,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E61" s="3">
         <v>0.47740000000000005</v>
@@ -30426,11 +31916,13 @@
       <c r="B62" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>231</v>
+      <c r="C62" s="2" t="str">
+        <f>VLOOKUP(A62,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Chemicals</v>
+      </c>
+      <c r="D62" s="2" t="str">
+        <f>VLOOKUP(A62,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E62" s="3">
         <v>0.17530000000000001</v>
@@ -30978,11 +32470,13 @@
       <c r="B63" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>231</v>
+      <c r="C63" s="2" t="str">
+        <f>VLOOKUP(A63,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Textiles, Apparel &amp; Luxury Goods</v>
+      </c>
+      <c r="D63" s="2" t="str">
+        <f>VLOOKUP(A63,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E63" s="3">
         <v>0.43959999999999999</v>
@@ -31462,11 +32956,13 @@
       <c r="B64" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>231</v>
+      <c r="C64" s="2" t="str">
+        <f>VLOOKUP(A64,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Hotels, Restaurants &amp; Leisure</v>
+      </c>
+      <c r="D64" s="2" t="str">
+        <f>VLOOKUP(A64,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E64" s="3">
         <v>-1.8799999999999997E-2</v>
@@ -32000,11 +33496,13 @@
       <c r="B65" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>231</v>
+      <c r="C65" s="2" t="str">
+        <f>VLOOKUP(A65,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D65" s="2" t="str">
+        <f>VLOOKUP(A65,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E65" s="3">
         <v>8.5989999999999997E-2</v>
@@ -32512,11 +34010,13 @@
       <c r="B66" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>231</v>
+      <c r="C66" s="2" t="str">
+        <f>VLOOKUP(A66,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Broadline Retail</v>
+      </c>
+      <c r="D66" s="2" t="str">
+        <f>VLOOKUP(A66,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E66" s="3">
         <v>0.40299000000000001</v>
@@ -32990,11 +34490,13 @@
       <c r="B67" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>231</v>
+      <c r="C67" s="2" t="str">
+        <f>VLOOKUP(A67,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Interactive Media &amp; Services</v>
+      </c>
+      <c r="D67" s="2" t="str">
+        <f>VLOOKUP(A67,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E67" s="3">
         <v>0.28039000000000003</v>
@@ -33408,11 +34910,13 @@
       <c r="B68" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>231</v>
+      <c r="C68" s="2" t="str">
+        <f>VLOOKUP(A68,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D68" s="2" t="str">
+        <f>VLOOKUP(A68,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E68" s="3">
         <v>0.40960000000000002</v>
@@ -33940,11 +35444,13 @@
       <c r="B69" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>231</v>
+      <c r="C69" s="2" t="str">
+        <f>VLOOKUP(A69,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D69" s="2" t="str">
+        <f>VLOOKUP(A69,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3">
@@ -34490,11 +35996,13 @@
       <c r="B70" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>231</v>
+      <c r="C70" s="2" t="str">
+        <f>VLOOKUP(A70,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D70" s="2" t="str">
+        <f>VLOOKUP(A70,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E70" s="3">
         <v>0.37130000000000002</v>
@@ -35022,11 +36530,13 @@
       <c r="B71" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>231</v>
+      <c r="C71" s="2" t="str">
+        <f>VLOOKUP(A71,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Biotechnology</v>
+      </c>
+      <c r="D71" s="2" t="str">
+        <f>VLOOKUP(A71,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E71" s="3">
         <v>-0.28588999999999998</v>
@@ -35324,11 +36834,13 @@
       <c r="B72" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>231</v>
+      <c r="C72" s="2" t="str">
+        <f>VLOOKUP(A72,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Food Products</v>
+      </c>
+      <c r="D72" s="2" t="str">
+        <f>VLOOKUP(A72,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E72" s="3">
         <v>0.1583</v>
@@ -35894,11 +37406,13 @@
       <c r="B73" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>260</v>
+      <c r="C73" s="2" t="str">
+        <f>VLOOKUP(A73,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Beverages</v>
+      </c>
+      <c r="D73" s="2" t="str">
+        <f>VLOOKUP(A73,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E73" s="3">
         <v>0.21600000000000003</v>
@@ -36398,11 +37912,13 @@
       <c r="B74" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>231</v>
+      <c r="C74" s="2" t="str">
+        <f>VLOOKUP(A74,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Entertainment</v>
+      </c>
+      <c r="D74" s="2" t="str">
+        <f>VLOOKUP(A74,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E74" s="3">
         <v>0.26149</v>
@@ -36928,11 +38444,13 @@
       <c r="B75" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>231</v>
+      <c r="C75" s="2" t="str">
+        <f>VLOOKUP(A75,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D75" s="2" t="str">
+        <f>VLOOKUP(A75,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E75" s="3">
         <v>0.99299000000000004</v>
@@ -37454,11 +38972,13 @@
       <c r="B76" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>231</v>
+      <c r="C76" s="2" t="str">
+        <f>VLOOKUP(A76,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D76" s="2" t="str">
+        <f>VLOOKUP(A76,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E76" s="3">
         <v>0.45500000000000002</v>
@@ -37886,11 +39406,13 @@
       <c r="B77" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>231</v>
+      <c r="C77" s="2" t="str">
+        <f>VLOOKUP(A77,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Specialty Retail</v>
+      </c>
+      <c r="D77" s="2" t="str">
+        <f>VLOOKUP(A77,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E77" s="3">
         <v>-1.6759999999999999</v>
@@ -38444,11 +39966,13 @@
       <c r="B78" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>231</v>
+      <c r="C78" s="2" t="str">
+        <f>VLOOKUP(A78,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Ground Transportation</v>
+      </c>
+      <c r="D78" s="2" t="str">
+        <f>VLOOKUP(A78,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E78" s="3">
         <v>0.31340000000000001</v>
@@ -38972,11 +40496,13 @@
       <c r="B79" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>231</v>
+      <c r="C79" s="2" t="str">
+        <f>VLOOKUP(A79,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D79" s="2" t="str">
+        <f>VLOOKUP(A79,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E79" s="3">
         <v>0.32289999999999996</v>
@@ -39490,11 +41016,13 @@
       <c r="B80" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>231</v>
+      <c r="C80" s="2" t="str">
+        <f>VLOOKUP(A80,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Machinery</v>
+      </c>
+      <c r="D80" s="2" t="str">
+        <f>VLOOKUP(A80,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E80" s="3">
         <v>0.31679999999999997</v>
@@ -40064,11 +41592,13 @@
       <c r="B81" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>231</v>
+      <c r="C81" s="2" t="str">
+        <f>VLOOKUP(A81,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D81" s="2" t="str">
+        <f>VLOOKUP(A81,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E81" s="3">
         <v>0.56320000000000003</v>
@@ -40470,11 +42000,13 @@
       <c r="B82" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>231</v>
+      <c r="C82" s="2" t="str">
+        <f>VLOOKUP(A82,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Professional Services</v>
+      </c>
+      <c r="D82" s="2" t="str">
+        <f>VLOOKUP(A82,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E82" s="3">
         <v>0.46859000000000001</v>
@@ -40994,11 +42526,13 @@
       <c r="B83" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>231</v>
+      <c r="C83" s="2" t="str">
+        <f>VLOOKUP(A83,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Financial Services</v>
+      </c>
+      <c r="D83" s="2" t="str">
+        <f>VLOOKUP(A83,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E83" s="3">
         <v>0.2732</v>
@@ -41382,11 +42916,13 @@
       <c r="B84" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>231</v>
+      <c r="C84" s="2" t="str">
+        <f>VLOOKUP(A84,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Broadline Retail</v>
+      </c>
+      <c r="D84" s="2" t="str">
+        <f>VLOOKUP(A84,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E84" s="3">
         <v>0.44520000000000004</v>
@@ -41692,11 +43228,13 @@
       <c r="B85" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>231</v>
+      <c r="C85" s="2" t="str">
+        <f>VLOOKUP(A85,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Beverages</v>
+      </c>
+      <c r="D85" s="2" t="str">
+        <f>VLOOKUP(A85,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E85" s="3">
         <v>0.59089999999999998</v>
@@ -42196,11 +43734,13 @@
       <c r="B86" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>231</v>
+      <c r="C86" s="2" t="str">
+        <f>VLOOKUP(A86,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D86" s="2" t="str">
+        <f>VLOOKUP(A86,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3">
@@ -42758,11 +44298,13 @@
       <c r="B87" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>231</v>
+      <c r="C87" s="2" t="str">
+        <f>VLOOKUP(A87,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Biotechnology</v>
+      </c>
+      <c r="D87" s="2" t="str">
+        <f>VLOOKUP(A87,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E87" s="3">
         <v>0.20699999999999999</v>
@@ -43290,11 +44832,13 @@
       <c r="B88" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>231</v>
+      <c r="C88" s="2" t="str">
+        <f>VLOOKUP(A88,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D88" s="2" t="str">
+        <f>VLOOKUP(A88,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E88" s="3">
         <v>0.1072</v>
@@ -43822,11 +45366,13 @@
       <c r="B89" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>231</v>
+      <c r="C89" s="2" t="str">
+        <f>VLOOKUP(A89,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Specialty Retail</v>
+      </c>
+      <c r="D89" s="2" t="str">
+        <f>VLOOKUP(A89,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E89" s="3">
         <v>0.40929000000000004</v>
@@ -44354,11 +45900,13 @@
       <c r="B90" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>231</v>
+      <c r="C90" s="2" t="str">
+        <f>VLOOKUP(A90,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Hotels, Restaurants &amp; Leisure</v>
+      </c>
+      <c r="D90" s="2" t="str">
+        <f>VLOOKUP(A90,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E90" s="3">
         <v>-0.48729999999999996</v>
@@ -44884,11 +46432,13 @@
       <c r="B91" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>231</v>
+      <c r="C91" s="2" t="str">
+        <f>VLOOKUP(A91,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Technology Hardware, Storage &amp; Peripherals</v>
+      </c>
+      <c r="D91" s="2" t="str">
+        <f>VLOOKUP(A91,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E91" s="3">
         <v>0.36149000000000003</v>
@@ -45308,11 +46858,13 @@
       <c r="B92" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>231</v>
+      <c r="C92" s="2" t="str">
+        <f>VLOOKUP(A92,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D92" s="2" t="str">
+        <f>VLOOKUP(A92,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E92" s="3">
         <v>0.29780000000000001</v>
@@ -45818,11 +47370,13 @@
       <c r="B93" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>231</v>
+      <c r="C93" s="2" t="str">
+        <f>VLOOKUP(A93,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Wireless Telecommunication Services</v>
+      </c>
+      <c r="D93" s="2" t="str">
+        <f>VLOOKUP(A93,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E93" s="3">
         <v>0.12380000000000001</v>
@@ -46290,11 +47844,13 @@
       <c r="B94" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>231</v>
+      <c r="C94" s="2" t="str">
+        <f>VLOOKUP(A94,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Entertainment</v>
+      </c>
+      <c r="D94" s="2" t="str">
+        <f>VLOOKUP(A94,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E94" s="3">
         <v>5.7800000000000004E-2</v>
@@ -46770,11 +48326,13 @@
       <c r="B95" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>231</v>
+      <c r="C95" s="2" t="str">
+        <f>VLOOKUP(A95,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Automobiles</v>
+      </c>
+      <c r="D95" s="2" t="str">
+        <f>VLOOKUP(A95,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E95" s="3">
         <v>0.20280000000000001</v>
@@ -47170,11 +48728,13 @@
       <c r="B96" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>231</v>
+      <c r="C96" s="2" t="str">
+        <f>VLOOKUP(A96,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="D96" s="2" t="str">
+        <f>VLOOKUP(A96,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E96" s="3">
         <v>0.41159000000000001</v>
@@ -47712,11 +49272,13 @@
       <c r="B97" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>231</v>
+      <c r="C97" s="2" t="str">
+        <f>VLOOKUP(A97,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Professional Services</v>
+      </c>
+      <c r="D97" s="2" t="str">
+        <f>VLOOKUP(A97,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E97" s="3">
         <v>0.81718999999999997</v>
@@ -48160,11 +49722,13 @@
       <c r="B98" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>260</v>
+      <c r="C98" s="2" t="str">
+        <f>VLOOKUP(A98,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Biotechnology</v>
+      </c>
+      <c r="D98" s="2" t="str">
+        <f>VLOOKUP(A98,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E98" s="3">
         <v>0.25198999999999999</v>
@@ -48650,11 +50214,13 @@
       <c r="B99" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>231</v>
+      <c r="C99" s="2" t="str">
+        <f>VLOOKUP(A99,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Entertainment</v>
+      </c>
+      <c r="D99" s="2" t="str">
+        <f>VLOOKUP(A99,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E99" s="3">
         <v>-6.7699999999999996E-2</v>
@@ -49126,11 +50692,13 @@
       <c r="B100" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>231</v>
+      <c r="C100" s="2" t="str">
+        <f>VLOOKUP(A100,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D100" s="2" t="str">
+        <f>VLOOKUP(A100,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E100" s="3">
         <v>0.22670000000000001</v>
@@ -49552,11 +51120,13 @@
       <c r="B101" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>231</v>
+      <c r="C101" s="2" t="str">
+        <f>VLOOKUP(A101,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Electric Utilities</v>
+      </c>
+      <c r="D101" s="2" t="str">
+        <f>VLOOKUP(A101,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E101" s="3">
         <v>0.10949</v>
@@ -50120,11 +51690,13 @@
       <c r="B102" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>231</v>
+      <c r="C102" s="2" t="str">
+        <f>VLOOKUP(A102,'[1]Current Screen Template'!$A:$D,4,FALSE)</f>
+        <v>Software</v>
+      </c>
+      <c r="D102" s="2" t="str">
+        <f>VLOOKUP(A102,'[1]Current Screen Template'!$A:$D,3,FALSE)</f>
+        <v>NASDAQ/NGS (GLOBAL SELECT MARKET)</v>
       </c>
       <c r="E102" s="3">
         <v>0.50968999999999998</v>
@@ -50446,12 +52018,8 @@
       <c r="GV102" s="4"/>
     </row>
     <row r="103" spans="1:204" x14ac:dyDescent="0.25">
-      <c r="C103" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>231</v>
-      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
       <c r="EO103" s="4">
         <v>46463000000</v>
       </c>
@@ -50534,12 +52102,8 @@
       <c r="GB103" s="4"/>
     </row>
     <row r="104" spans="1:204" x14ac:dyDescent="0.25">
-      <c r="C104" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>231</v>
-      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
       <c r="EO104" s="4">
         <v>3430866000</v>
       </c>
@@ -50691,6 +52255,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="BM1:CF1"/>
+    <mergeCell ref="CG1:CZ1"/>
+    <mergeCell ref="DA1:DT1"/>
+    <mergeCell ref="DU1:EN1"/>
+    <mergeCell ref="GC1:GV1"/>
+    <mergeCell ref="EO1:FH1"/>
+    <mergeCell ref="FI1:GB1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="E1:X1"/>
@@ -50698,13 +52269,6 @@
     <mergeCell ref="AS1:BL1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="BM1:CF1"/>
-    <mergeCell ref="CG1:CZ1"/>
-    <mergeCell ref="DA1:DT1"/>
-    <mergeCell ref="DU1:EN1"/>
-    <mergeCell ref="GC1:GV1"/>
-    <mergeCell ref="EO1:FH1"/>
-    <mergeCell ref="FI1:GB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>